<commit_message>
Refactor timetable generation: Replace Excel mappings with CSV files for student and group data, update timetable generation logic, and remove obsolete files.
</commit_message>
<xml_diff>
--- a/flute-time-table.xlsx
+++ b/flute-time-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Python\summer-camp-time-table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796662C1-1454-40EF-A3DF-E931E9B04F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55CCA59-6E4A-461D-A796-260A5EA780D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="585" windowWidth="17085" windowHeight="13425" activeTab="1" xr2:uid="{4F305ACA-9255-4D6C-9A65-1407DE2CF383}"/>
+    <workbookView xWindow="5370" yWindow="1245" windowWidth="17085" windowHeight="13425" xr2:uid="{4F305ACA-9255-4D6C-9A65-1407DE2CF383}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="49">
   <si>
     <t xml:space="preserve">Time </t>
   </si>
@@ -164,9 +164,6 @@
 Maritime Museum Tour</t>
   </si>
   <si>
-    <t>Rehearsal for Students and Friends Concert</t>
-  </si>
-  <si>
     <t>Lunch
 Dress Up, Warm Up</t>
   </si>
@@ -180,6 +177,25 @@
   <si>
     <t>F1 Rehearsal with pianist
  Shelley's Room</t>
+  </si>
+  <si>
+    <t>Rehearsal for Students and Friend's Concert</t>
+  </si>
+  <si>
+    <t>Rehearsal for Faculty Concert</t>
+  </si>
+  <si>
+    <t>Break</t>
+  </si>
+  <si>
+    <t>Lina Summer Camp of Music Faculty Concert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After concert refreshment </t>
+  </si>
+  <si>
+    <t>After Concert Dinner 
+(Mandarin Oriental Private Room)</t>
   </si>
 </sst>
 </file>
@@ -248,7 +264,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -475,11 +491,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -660,22 +711,34 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -694,24 +757,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1059,7 +1104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58029A68-0D30-435A-A4C3-6E59A3275874}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="C13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
       <selection activeCell="D28" sqref="D28:D31"/>
     </sheetView>
   </sheetViews>
@@ -1203,7 +1248,7 @@
         <v>6</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="33" t="s">
         <v>8</v>
@@ -1572,7 +1617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85528851-3886-44FD-9E54-783F0AC6C099}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="D28" sqref="D28:D31"/>
     </sheetView>
   </sheetViews>
@@ -3547,21 +3592,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F258A27A-E0BD-410A-AC93-E998D70178A7}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20:E25"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="6" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3571,12 +3615,8 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1">
       <c r="A2" s="4">
         <v>0.41666666666666669</v>
       </c>
@@ -3584,267 +3624,408 @@
         <v>38</v>
       </c>
       <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-    </row>
-    <row r="3" spans="1:5">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="4">
         <v>0.42708333333333331</v>
       </c>
       <c r="B3" s="54"/>
       <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-    </row>
-    <row r="4" spans="1:5">
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="4">
         <v>0.4375</v>
       </c>
       <c r="B4" s="54"/>
       <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-    </row>
-    <row r="5" spans="1:5">
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="4">
         <v>0.44791666666666702</v>
       </c>
       <c r="B5" s="54"/>
       <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-    </row>
-    <row r="6" spans="1:5">
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1">
       <c r="A6" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B6" s="76" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="77"/>
-      <c r="D6" s="82" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="83"/>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="B6" s="80" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="81"/>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="85"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="B7" s="82"/>
+      <c r="C7" s="83"/>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B8" s="78"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="85"/>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="B8" s="82"/>
+      <c r="C8" s="83"/>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B9" s="78"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="85"/>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="B9" s="82"/>
+      <c r="C9" s="83"/>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="4">
         <v>0.5</v>
       </c>
-      <c r="B10" s="78"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="85"/>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="B10" s="82"/>
+      <c r="C10" s="83"/>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="85"/>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="B11" s="82"/>
+      <c r="C11" s="83"/>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B12" s="78"/>
-      <c r="C12" s="79"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="85"/>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="B12" s="82"/>
+      <c r="C12" s="83"/>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="87"/>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="B13" s="84"/>
+      <c r="C13" s="85"/>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1">
       <c r="A14" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B14" s="88" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="89"/>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="B14" s="86" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="87"/>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B15" s="90"/>
+      <c r="B15" s="88"/>
       <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-    </row>
-    <row r="16" spans="1:5">
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B16" s="90"/>
+      <c r="B16" s="88"/>
       <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-    </row>
-    <row r="17" spans="1:5">
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B17" s="90"/>
+      <c r="B17" s="88"/>
       <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-    </row>
-    <row r="18" spans="1:5">
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B18" s="90"/>
+      <c r="B18" s="88"/>
       <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-    </row>
-    <row r="19" spans="1:5">
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B19" s="90"/>
+      <c r="B19" s="88"/>
       <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-    </row>
-    <row r="20" spans="1:5">
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1">
       <c r="A20" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B20" s="76" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="77"/>
-      <c r="D20" s="70" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="71"/>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="B20" s="80" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="81"/>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B21" s="78"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="73"/>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="B21" s="82"/>
+      <c r="C21" s="83"/>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="4">
         <v>0.625</v>
       </c>
-      <c r="B22" s="78"/>
-      <c r="C22" s="79"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="73"/>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="B22" s="82"/>
+      <c r="C22" s="83"/>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B23" s="78"/>
-      <c r="C23" s="79"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="73"/>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="B23" s="82"/>
+      <c r="C23" s="83"/>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B24" s="78"/>
-      <c r="C24" s="79"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="73"/>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="B24" s="82"/>
+      <c r="C24" s="83"/>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B25" s="78"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="75"/>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="B25" s="82"/>
+      <c r="C25" s="83"/>
+    </row>
+    <row r="26" spans="1:3" ht="15" customHeight="1">
       <c r="A26" s="4">
         <v>0.66666666666666696</v>
       </c>
       <c r="B26" s="64" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="65"/>
-      <c r="D26" s="70" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" s="71"/>
-    </row>
-    <row r="27" spans="1:5">
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="4">
         <v>0.67708333333333304</v>
       </c>
       <c r="B27" s="66"/>
       <c r="C27" s="67"/>
-      <c r="D27" s="72"/>
-      <c r="E27" s="73"/>
-    </row>
-    <row r="28" spans="1:5">
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="4">
         <v>0.6875</v>
       </c>
       <c r="B28" s="68"/>
       <c r="C28" s="69"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="75"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="4">
+        <v>0.69791666666666696</v>
+      </c>
+      <c r="B29" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="65"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="4">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="B30" s="66"/>
+      <c r="C30" s="67"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="4">
+        <v>0.718749999999999</v>
+      </c>
+      <c r="B31" s="68"/>
+      <c r="C31" s="69"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="4">
+        <v>0.72916666666666496</v>
+      </c>
+      <c r="B32" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="71"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="4">
+        <v>0.73958333333333104</v>
+      </c>
+      <c r="B33" s="72"/>
+      <c r="C33" s="73"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="4">
+        <v>0.749999999999997</v>
+      </c>
+      <c r="B34" s="72"/>
+      <c r="C34" s="73"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="4">
+        <v>0.76041666666666297</v>
+      </c>
+      <c r="B35" s="74"/>
+      <c r="C35" s="75"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="4">
+        <v>0.77083333333332904</v>
+      </c>
+      <c r="B36" s="76" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="76"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="4">
+        <v>0.781249999999996</v>
+      </c>
+      <c r="B37" s="77"/>
+      <c r="C37" s="77"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="4">
+        <v>0.79166666666666197</v>
+      </c>
+      <c r="B38" s="77"/>
+      <c r="C38" s="77"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="4">
+        <v>0.80208333333332804</v>
+      </c>
+      <c r="B39" s="77"/>
+      <c r="C39" s="77"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="4">
+        <v>0.812499999999994</v>
+      </c>
+      <c r="B40" s="77"/>
+      <c r="C40" s="77"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="4">
+        <v>0.82291666666665997</v>
+      </c>
+      <c r="B41" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="71"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="4">
+        <v>0.83333333333332604</v>
+      </c>
+      <c r="B42" s="72"/>
+      <c r="C42" s="73"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="4">
+        <v>0.84374999999999201</v>
+      </c>
+      <c r="B43" s="72"/>
+      <c r="C43" s="73"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="4">
+        <v>0.85416666666665797</v>
+      </c>
+      <c r="B44" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="79"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="4">
+        <v>0.86458333333332404</v>
+      </c>
+      <c r="B45" s="68"/>
+      <c r="C45" s="69"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="4">
+        <v>0.87499999999999001</v>
+      </c>
+      <c r="B46" s="68"/>
+      <c r="C46" s="69"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="4">
+        <v>0.88541666666665597</v>
+      </c>
+      <c r="B47" s="68"/>
+      <c r="C47" s="69"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="4">
+        <v>0.89583333333332205</v>
+      </c>
+      <c r="B48" s="68"/>
+      <c r="C48" s="69"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="4">
+        <v>0.90624999999998801</v>
+      </c>
+      <c r="B49" s="68"/>
+      <c r="C49" s="69"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="4">
+        <v>0.91666666666665497</v>
+      </c>
+      <c r="B50" s="68"/>
+      <c r="C50" s="69"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="4">
+        <v>0.92708333333332105</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="4">
+        <v>0.93749999999998701</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="4">
+        <v>0.94791666666665297</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="4">
+        <v>0.95833333333331905</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="4">
+        <v>0.96874999999998501</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="4">
+        <v>0.97916666666665098</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="4">
+        <v>0.98958333333331705</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="B2:C5"/>
+    <mergeCell ref="B6:C13"/>
+    <mergeCell ref="B14:C19"/>
+    <mergeCell ref="B20:C25"/>
     <mergeCell ref="B26:C28"/>
-    <mergeCell ref="D26:E28"/>
-    <mergeCell ref="B2:E5"/>
-    <mergeCell ref="B6:C13"/>
-    <mergeCell ref="D6:E13"/>
-    <mergeCell ref="B14:E19"/>
-    <mergeCell ref="B20:C25"/>
-    <mergeCell ref="D20:E25"/>
+    <mergeCell ref="B29:C31"/>
+    <mergeCell ref="B32:C35"/>
+    <mergeCell ref="B36:C40"/>
+    <mergeCell ref="B41:C43"/>
+    <mergeCell ref="B44:C50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update timetable generation logic to improve activity descriptions and remove unnecessary student timetable files.
</commit_message>
<xml_diff>
--- a/flute-time-table.xlsx
+++ b/flute-time-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Python\summer-camp-time-table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55CCA59-6E4A-461D-A796-260A5EA780D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDBB5BD-1FA8-46F9-BBEA-3CB0DBC7F168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5370" yWindow="1245" windowWidth="17085" windowHeight="13425" xr2:uid="{4F305ACA-9255-4D6C-9A65-1407DE2CF383}"/>
+    <workbookView xWindow="645" yWindow="915" windowWidth="17085" windowHeight="13425" xr2:uid="{4F305ACA-9255-4D6C-9A65-1407DE2CF383}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="1" r:id="rId1"/>
@@ -159,11 +159,6 @@
     <t>Master class with Ivy &amp; Stephane</t>
   </si>
   <si>
-    <t>Check in Maritime Time
-Briefing for Saturday Concert 
-Maritime Museum Tour</t>
-  </si>
-  <si>
     <t>Lunch
 Dress Up, Warm Up</t>
   </si>
@@ -196,6 +191,11 @@
   <si>
     <t>After Concert Dinner 
 (Mandarin Oriental Private Room)</t>
+  </si>
+  <si>
+    <t>Check in Maritime Time
+Briefing 
+Maritime Museum Tour</t>
   </si>
 </sst>
 </file>
@@ -555,25 +555,40 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -583,7 +598,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -598,65 +613,50 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -693,6 +693,33 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -739,33 +766,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1104,7 +1104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58029A68-0D30-435A-A4C3-6E59A3275874}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D28" sqref="D28:D31"/>
     </sheetView>
   </sheetViews>
@@ -1139,68 +1139,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="33" t="s">
+      <c r="G7" s="19" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1241,22 +1241,22 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="33" t="s">
+      <c r="D11" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="G11" s="19" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1267,7 +1267,7 @@
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="34"/>
+      <c r="E12" s="23"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
     </row>
@@ -1278,7 +1278,7 @@
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="34"/>
+      <c r="E13" s="23"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
     </row>
@@ -1289,7 +1289,7 @@
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
-      <c r="E14" s="35"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
     </row>
@@ -1297,69 +1297,69 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="G20" s="19" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1400,18 +1400,18 @@
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="4">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="18"/>
+      <c r="D25" s="38"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
@@ -1430,7 +1430,7 @@
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="18"/>
+      <c r="D26" s="38"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
-      <c r="D27" s="19"/>
+      <c r="D27" s="39"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -1450,26 +1450,26 @@
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
       <c r="B29" s="13"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
@@ -1479,8 +1479,8 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="13"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
@@ -1490,8 +1490,8 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B31" s="14"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -1509,10 +1509,10 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="7"/>
@@ -1574,6 +1574,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="C33:C39"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="B15:E19"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
     <mergeCell ref="F24:F27"/>
     <mergeCell ref="G24:G27"/>
     <mergeCell ref="F28:F31"/>
@@ -1590,24 +1608,6 @@
     <mergeCell ref="D20:D23"/>
     <mergeCell ref="E20:E23"/>
     <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="B15:E19"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="B33:B39"/>
-    <mergeCell ref="C33:C39"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D24:D27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1617,7 +1617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85528851-3886-44FD-9E54-783F0AC6C099}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="D28" sqref="D28:D31"/>
     </sheetView>
   </sheetViews>
@@ -1650,68 +1650,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="33" t="s">
+      <c r="G7" s="19" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1720,7 +1720,7 @@
         <v>0.46875</v>
       </c>
       <c r="B8" s="13"/>
-      <c r="C8" s="42"/>
+      <c r="C8" s="40"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
@@ -1731,7 +1731,7 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B9" s="13"/>
-      <c r="C9" s="42"/>
+      <c r="C9" s="40"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -1742,7 +1742,7 @@
         <v>0.48958333333333298</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="43"/>
+      <c r="C10" s="41"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -1752,22 +1752,22 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="G11" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1776,7 +1776,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="B12" s="13"/>
-      <c r="C12" s="42"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
@@ -1787,7 +1787,7 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B13" s="13"/>
-      <c r="C13" s="42"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
@@ -1798,7 +1798,7 @@
         <v>0.53125</v>
       </c>
       <c r="B14" s="14"/>
-      <c r="C14" s="43"/>
+      <c r="C14" s="41"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -1808,79 +1808,79 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="47"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="26" t="s">
+      <c r="E20" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="26" t="s">
+      <c r="G20" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1889,7 +1889,7 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B21" s="13"/>
-      <c r="C21" s="42"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
@@ -1900,7 +1900,7 @@
         <v>0.61458333333333304</v>
       </c>
       <c r="B22" s="13"/>
-      <c r="C22" s="42"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
@@ -1911,7 +1911,7 @@
         <v>0.625</v>
       </c>
       <c r="B23" s="14"/>
-      <c r="C23" s="43"/>
+      <c r="C23" s="41"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
@@ -1921,26 +1921,26 @@
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="4">
         <v>0.64583333333333304</v>
       </c>
       <c r="B25" s="13"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="28"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="33"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
@@ -1950,8 +1950,8 @@
         <v>0.65625</v>
       </c>
       <c r="B26" s="13"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="28"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="33"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
@@ -1961,8 +1961,8 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="B27" s="14"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="29"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="34"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -1971,26 +1971,26 @@
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
       <c r="B29" s="13"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="28"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="33"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
@@ -2000,8 +2000,8 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="13"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="28"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="33"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
@@ -2011,8 +2011,8 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B31" s="14"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="29"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="34"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -2032,10 +2032,10 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="7"/>
@@ -2048,7 +2048,7 @@
         <v>0.73958333333333104</v>
       </c>
       <c r="B34" s="13"/>
-      <c r="C34" s="42"/>
+      <c r="C34" s="40"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -2059,7 +2059,7 @@
         <v>0.749999999999997</v>
       </c>
       <c r="B35" s="13"/>
-      <c r="C35" s="42"/>
+      <c r="C35" s="40"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -2070,7 +2070,7 @@
         <v>0.76041666666666297</v>
       </c>
       <c r="B36" s="13"/>
-      <c r="C36" s="42"/>
+      <c r="C36" s="40"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2081,7 +2081,7 @@
         <v>0.77083333333332904</v>
       </c>
       <c r="B37" s="13"/>
-      <c r="C37" s="42"/>
+      <c r="C37" s="40"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -2092,7 +2092,7 @@
         <v>0.781249999999996</v>
       </c>
       <c r="B38" s="13"/>
-      <c r="C38" s="42"/>
+      <c r="C38" s="40"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -2103,7 +2103,7 @@
         <v>0.79166666666666197</v>
       </c>
       <c r="B39" s="14"/>
-      <c r="C39" s="43"/>
+      <c r="C39" s="41"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
@@ -2111,6 +2111,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
     <mergeCell ref="F28:F31"/>
     <mergeCell ref="G28:G31"/>
     <mergeCell ref="B33:B39"/>
@@ -2127,24 +2145,6 @@
     <mergeCell ref="G24:G27"/>
     <mergeCell ref="F7:F10"/>
     <mergeCell ref="G7:G10"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="E28:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2187,61 +2187,61 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2279,19 +2279,19 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="19" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2329,71 +2329,71 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="47"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="26" t="s">
+      <c r="E20" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="19" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2431,16 +2431,16 @@
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="26"/>
+      <c r="E24" s="12"/>
       <c r="F24" s="10"/>
     </row>
     <row r="25" spans="1:6">
@@ -2477,16 +2477,16 @@
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="26"/>
+      <c r="E28" s="12"/>
       <c r="F28" s="10"/>
     </row>
     <row r="29" spans="1:6">
@@ -2494,7 +2494,7 @@
         <v>0.6875</v>
       </c>
       <c r="B29" s="13"/>
-      <c r="C29" s="28"/>
+      <c r="C29" s="33"/>
       <c r="D29" s="51"/>
       <c r="E29" s="13"/>
       <c r="F29" s="8"/>
@@ -2504,7 +2504,7 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="13"/>
-      <c r="C30" s="28"/>
+      <c r="C30" s="33"/>
       <c r="D30" s="51"/>
       <c r="E30" s="13"/>
       <c r="F30" s="8"/>
@@ -2514,7 +2514,7 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B31" s="14"/>
-      <c r="C31" s="29"/>
+      <c r="C31" s="34"/>
       <c r="D31" s="52"/>
       <c r="E31" s="14"/>
       <c r="F31" s="8"/>
@@ -2533,10 +2533,10 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="7"/>
@@ -2605,6 +2605,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="C33:C39"/>
     <mergeCell ref="B3:F6"/>
     <mergeCell ref="B15:F19"/>
     <mergeCell ref="F20:F23"/>
@@ -2621,17 +2632,6 @@
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="C20:C23"/>
     <mergeCell ref="D20:D23"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="B33:B39"/>
-    <mergeCell ref="C33:C39"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2678,68 +2678,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="12" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2748,7 +2748,7 @@
         <v>0.46875</v>
       </c>
       <c r="B8" s="13"/>
-      <c r="C8" s="28"/>
+      <c r="C8" s="33"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
@@ -2759,7 +2759,7 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B9" s="13"/>
-      <c r="C9" s="28"/>
+      <c r="C9" s="33"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -2770,7 +2770,7 @@
         <v>0.48958333333333298</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="29"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -2780,22 +2780,22 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="G11" s="12" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2804,7 +2804,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="B12" s="13"/>
-      <c r="C12" s="28"/>
+      <c r="C12" s="33"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
@@ -2815,7 +2815,7 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B13" s="13"/>
-      <c r="C13" s="28"/>
+      <c r="C13" s="33"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
@@ -2826,7 +2826,7 @@
         <v>0.53125</v>
       </c>
       <c r="B14" s="14"/>
-      <c r="C14" s="29"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -2836,79 +2836,79 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="47"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="G20" s="19" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2917,7 +2917,7 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B21" s="13"/>
-      <c r="C21" s="28"/>
+      <c r="C21" s="33"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
@@ -2928,7 +2928,7 @@
         <v>0.61458333333333304</v>
       </c>
       <c r="B22" s="13"/>
-      <c r="C22" s="28"/>
+      <c r="C22" s="33"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
@@ -2939,7 +2939,7 @@
         <v>0.625</v>
       </c>
       <c r="B23" s="14"/>
-      <c r="C23" s="29"/>
+      <c r="C23" s="34"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
@@ -2949,18 +2949,18 @@
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="4">
@@ -2968,7 +2968,7 @@
       </c>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="28"/>
+      <c r="D25" s="33"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
@@ -2979,7 +2979,7 @@
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="28"/>
+      <c r="D26" s="33"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
@@ -2990,7 +2990,7 @@
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
-      <c r="D27" s="29"/>
+      <c r="D27" s="34"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -2999,26 +2999,26 @@
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
       <c r="B29" s="13"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
@@ -3028,8 +3028,8 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="13"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
@@ -3039,8 +3039,8 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B31" s="14"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -3060,10 +3060,10 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="7"/>
@@ -3139,6 +3139,27 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="C33:C39"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="B15:G19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="G20:G23"/>
     <mergeCell ref="G11:G14"/>
     <mergeCell ref="B3:G6"/>
     <mergeCell ref="B7:B10"/>
@@ -3152,27 +3173,6 @@
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="F11:F14"/>
-    <mergeCell ref="B15:G19"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="G28:G31"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="B33:B39"/>
-    <mergeCell ref="C33:C39"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D28:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3216,7 +3216,7 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="42" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="53"/>
@@ -3228,27 +3228,27 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="B4" s="54"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
       <c r="B5" s="54"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
       <c r="B6" s="54"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="4">
@@ -3328,48 +3328,48 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="4">
@@ -3413,16 +3413,16 @@
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="26"/>
+      <c r="E24" s="12"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="4">
@@ -3430,7 +3430,7 @@
       </c>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="28"/>
+      <c r="D25" s="33"/>
       <c r="E25" s="13"/>
     </row>
     <row r="26" spans="1:5">
@@ -3439,7 +3439,7 @@
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="28"/>
+      <c r="D26" s="33"/>
       <c r="E26" s="13"/>
     </row>
     <row r="27" spans="1:5">
@@ -3448,31 +3448,31 @@
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
-      <c r="D27" s="29"/>
+      <c r="D27" s="34"/>
       <c r="E27" s="14"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="26"/>
+      <c r="E28" s="12"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
       <c r="B29" s="13"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
       <c r="E29" s="13"/>
     </row>
     <row r="30" spans="1:5">
@@ -3480,8 +3480,8 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="13"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
       <c r="E30" s="13"/>
     </row>
     <row r="31" spans="1:5">
@@ -3489,8 +3489,8 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B31" s="14"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
       <c r="E31" s="14"/>
     </row>
     <row r="32" spans="1:5">
@@ -3506,10 +3506,10 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="7"/>
@@ -3571,6 +3571,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="C33:C39"/>
     <mergeCell ref="B3:E6"/>
     <mergeCell ref="B7:E14"/>
     <mergeCell ref="B15:E19"/>
@@ -3579,12 +3585,6 @@
     <mergeCell ref="C24:C27"/>
     <mergeCell ref="D24:D27"/>
     <mergeCell ref="E24:E27"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="B33:B39"/>
-    <mergeCell ref="C33:C39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3594,8 +3594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F258A27A-E0BD-410A-AC93-E998D70178A7}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3620,8 +3620,8 @@
       <c r="A2" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B2" s="44" t="s">
-        <v>38</v>
+      <c r="B2" s="42" t="s">
+        <v>48</v>
       </c>
       <c r="C2" s="53"/>
     </row>
@@ -3630,354 +3630,354 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="B3" s="54"/>
-      <c r="C3" s="23"/>
+      <c r="C3" s="28"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4">
         <v>0.4375</v>
       </c>
       <c r="B4" s="54"/>
-      <c r="C4" s="23"/>
+      <c r="C4" s="28"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4">
         <v>0.44791666666666702</v>
       </c>
       <c r="B5" s="54"/>
-      <c r="C5" s="23"/>
+      <c r="C5" s="28"/>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1">
       <c r="A6" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B6" s="80" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="81"/>
+      <c r="B6" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="65"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="83"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="67"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B8" s="82"/>
-      <c r="C8" s="83"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="67"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B9" s="82"/>
-      <c r="C9" s="83"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="67"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4">
         <v>0.5</v>
       </c>
-      <c r="B10" s="82"/>
-      <c r="C10" s="83"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="67"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B11" s="82"/>
-      <c r="C11" s="83"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="67"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B12" s="82"/>
-      <c r="C12" s="83"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="67"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B13" s="84"/>
-      <c r="C13" s="85"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="69"/>
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1">
       <c r="A14" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B14" s="86" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="87"/>
+      <c r="B14" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="71"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B15" s="88"/>
-      <c r="C15" s="37"/>
+      <c r="B15" s="72"/>
+      <c r="C15" s="16"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B16" s="88"/>
-      <c r="C16" s="37"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="16"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B17" s="88"/>
-      <c r="C17" s="37"/>
+      <c r="B17" s="72"/>
+      <c r="C17" s="16"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B18" s="88"/>
-      <c r="C18" s="37"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B19" s="88"/>
-      <c r="C19" s="37"/>
+      <c r="B19" s="72"/>
+      <c r="C19" s="16"/>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1">
       <c r="A20" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B20" s="80" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="81"/>
+      <c r="B20" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="65"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B21" s="82"/>
-      <c r="C21" s="83"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="67"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="4">
         <v>0.625</v>
       </c>
-      <c r="B22" s="82"/>
-      <c r="C22" s="83"/>
+      <c r="B22" s="66"/>
+      <c r="C22" s="67"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B23" s="82"/>
-      <c r="C23" s="83"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="67"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B24" s="82"/>
-      <c r="C24" s="83"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="67"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B25" s="82"/>
-      <c r="C25" s="83"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="67"/>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1">
       <c r="A26" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B26" s="64" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="65"/>
+      <c r="B26" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="74"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B27" s="66"/>
-      <c r="C27" s="67"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="76"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="4">
         <v>0.6875</v>
       </c>
-      <c r="B28" s="68"/>
-      <c r="C28" s="69"/>
+      <c r="B28" s="77"/>
+      <c r="C28" s="78"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="4">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B29" s="64" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="65"/>
+      <c r="B29" s="73" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="74"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="4">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B30" s="66"/>
-      <c r="C30" s="67"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="76"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B31" s="68"/>
-      <c r="C31" s="69"/>
+      <c r="B31" s="77"/>
+      <c r="C31" s="78"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B32" s="70" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="71"/>
+      <c r="B32" s="79" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="80"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B33" s="72"/>
-      <c r="C33" s="73"/>
+      <c r="B33" s="81"/>
+      <c r="C33" s="82"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B34" s="72"/>
-      <c r="C34" s="73"/>
+      <c r="B34" s="81"/>
+      <c r="C34" s="82"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B35" s="74"/>
-      <c r="C35" s="75"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="84"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B36" s="76" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="76"/>
+      <c r="B36" s="85" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="85"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B37" s="77"/>
-      <c r="C37" s="77"/>
+      <c r="B37" s="86"/>
+      <c r="C37" s="86"/>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="4">
         <v>0.79166666666666197</v>
       </c>
-      <c r="B38" s="77"/>
-      <c r="C38" s="77"/>
+      <c r="B38" s="86"/>
+      <c r="C38" s="86"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="4">
         <v>0.80208333333332804</v>
       </c>
-      <c r="B39" s="77"/>
-      <c r="C39" s="77"/>
+      <c r="B39" s="86"/>
+      <c r="C39" s="86"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="4">
         <v>0.812499999999994</v>
       </c>
-      <c r="B40" s="77"/>
-      <c r="C40" s="77"/>
+      <c r="B40" s="86"/>
+      <c r="C40" s="86"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="4">
         <v>0.82291666666665997</v>
       </c>
-      <c r="B41" s="70" t="s">
-        <v>47</v>
-      </c>
-      <c r="C41" s="71"/>
+      <c r="B41" s="79" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="80"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="4">
         <v>0.83333333333332604</v>
       </c>
-      <c r="B42" s="72"/>
-      <c r="C42" s="73"/>
+      <c r="B42" s="81"/>
+      <c r="C42" s="82"/>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="4">
         <v>0.84374999999999201</v>
       </c>
-      <c r="B43" s="72"/>
-      <c r="C43" s="73"/>
+      <c r="B43" s="81"/>
+      <c r="C43" s="82"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="4">
         <v>0.85416666666665797</v>
       </c>
-      <c r="B44" s="78" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" s="79"/>
+      <c r="B44" s="87" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="88"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="4">
         <v>0.86458333333332404</v>
       </c>
-      <c r="B45" s="68"/>
-      <c r="C45" s="69"/>
+      <c r="B45" s="77"/>
+      <c r="C45" s="78"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="4">
         <v>0.87499999999999001</v>
       </c>
-      <c r="B46" s="68"/>
-      <c r="C46" s="69"/>
+      <c r="B46" s="77"/>
+      <c r="C46" s="78"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="4">
         <v>0.88541666666665597</v>
       </c>
-      <c r="B47" s="68"/>
-      <c r="C47" s="69"/>
+      <c r="B47" s="77"/>
+      <c r="C47" s="78"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="4">
         <v>0.89583333333332205</v>
       </c>
-      <c r="B48" s="68"/>
-      <c r="C48" s="69"/>
+      <c r="B48" s="77"/>
+      <c r="C48" s="78"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="4">
         <v>0.90624999999998801</v>
       </c>
-      <c r="B49" s="68"/>
-      <c r="C49" s="69"/>
+      <c r="B49" s="77"/>
+      <c r="C49" s="78"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="4">
         <v>0.91666666666665497</v>
       </c>
-      <c r="B50" s="68"/>
-      <c r="C50" s="69"/>
+      <c r="B50" s="77"/>
+      <c r="C50" s="78"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="4">
@@ -4016,16 +4016,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B29:C31"/>
+    <mergeCell ref="B32:C35"/>
+    <mergeCell ref="B36:C40"/>
+    <mergeCell ref="B41:C43"/>
+    <mergeCell ref="B44:C50"/>
     <mergeCell ref="B2:C5"/>
     <mergeCell ref="B6:C13"/>
     <mergeCell ref="B14:C19"/>
     <mergeCell ref="B20:C25"/>
     <mergeCell ref="B26:C28"/>
-    <mergeCell ref="B29:C31"/>
-    <mergeCell ref="B32:C35"/>
-    <mergeCell ref="B36:C40"/>
-    <mergeCell ref="B41:C43"/>
-    <mergeCell ref="B44:C50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update timetable generation logic to exclude activities after 17:00 for Days 1-5 and enhance activity selection for student schedules. Update related timetable files.
</commit_message>
<xml_diff>
--- a/flute-time-table.xlsx
+++ b/flute-time-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Python\summer-camp-time-table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDBB5BD-1FA8-46F9-BBEA-3CB0DBC7F168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB06778-3AF9-48C4-98DA-FEA9281B254F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="915" windowWidth="17085" windowHeight="13425" xr2:uid="{4F305ACA-9255-4D6C-9A65-1407DE2CF383}"/>
+    <workbookView xWindow="30" yWindow="825" windowWidth="17085" windowHeight="13425" xr2:uid="{4F305ACA-9255-4D6C-9A65-1407DE2CF383}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="1" r:id="rId1"/>
@@ -46,12 +46,6 @@
     <t xml:space="preserve">Time </t>
   </si>
   <si>
-    <t>CHUANG, Ivy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETY, Stephane </t>
-  </si>
-  <si>
     <t>Welcome Speech</t>
   </si>
   <si>
@@ -196,6 +190,12 @@
     <t>Check in Maritime Time
 Briefing 
 Maritime Museum Tour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivy CHUANG </t>
+  </si>
+  <si>
+    <t>Stephane RETY</t>
   </si>
 </sst>
 </file>
@@ -555,40 +555,25 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -598,7 +583,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -613,16 +598,37 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -651,12 +657,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -693,6 +693,54 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -718,54 +766,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1104,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58029A68-0D30-435A-A4C3-6E59A3275874}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28:D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1119,13 +1119,13 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1139,69 +1139,69 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
+      <c r="B3" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="G7" s="33" t="s">
         <v>5</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1241,23 +1241,23 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>5</v>
+      <c r="G11" s="33" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1267,7 +1267,7 @@
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="23"/>
+      <c r="E12" s="34"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
     </row>
@@ -1278,7 +1278,7 @@
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="23"/>
+      <c r="E13" s="34"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
     </row>
@@ -1289,7 +1289,7 @@
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
-      <c r="E14" s="24"/>
+      <c r="E14" s="35"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
     </row>
@@ -1297,70 +1297,70 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
+      <c r="B15" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="19" t="s">
+      <c r="B20" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="19" t="s">
-        <v>5</v>
+      <c r="G20" s="33" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1400,18 +1400,18 @@
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="4">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="38"/>
+      <c r="D25" s="18"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
@@ -1430,7 +1430,7 @@
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="38"/>
+      <c r="D26" s="18"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
-      <c r="D27" s="39"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -1450,26 +1450,26 @@
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
+      <c r="B28" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
       <c r="B29" s="13"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
@@ -1479,8 +1479,8 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="13"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
@@ -1490,8 +1490,8 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B31" s="14"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -1509,11 +1509,11 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="37" t="s">
-        <v>11</v>
+      <c r="B33" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -1574,24 +1574,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B33:B39"/>
-    <mergeCell ref="C33:C39"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="B15:E19"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
     <mergeCell ref="F24:F27"/>
     <mergeCell ref="G24:G27"/>
     <mergeCell ref="F28:F31"/>
@@ -1608,6 +1590,24 @@
     <mergeCell ref="D20:D23"/>
     <mergeCell ref="E20:E23"/>
     <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="B15:E19"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="C33:C39"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="D24:D27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1617,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85528851-3886-44FD-9E54-783F0AC6C099}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28:D31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1632,13 +1632,13 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1">
@@ -1650,69 +1650,69 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
+      <c r="B3" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="50" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>9</v>
+      <c r="G7" s="33" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1720,7 +1720,7 @@
         <v>0.46875</v>
       </c>
       <c r="B8" s="13"/>
-      <c r="C8" s="40"/>
+      <c r="C8" s="42"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
@@ -1731,7 +1731,7 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B9" s="13"/>
-      <c r="C9" s="40"/>
+      <c r="C9" s="42"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -1742,7 +1742,7 @@
         <v>0.48958333333333298</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="41"/>
+      <c r="C10" s="43"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -1752,23 +1752,23 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="49" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="50" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="12" t="s">
+      <c r="B11" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="G11" s="26" t="s">
         <v>4</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1776,7 +1776,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="B12" s="13"/>
-      <c r="C12" s="40"/>
+      <c r="C12" s="42"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
@@ -1787,7 +1787,7 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B13" s="13"/>
-      <c r="C13" s="40"/>
+      <c r="C13" s="42"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
@@ -1798,7 +1798,7 @@
         <v>0.53125</v>
       </c>
       <c r="B14" s="14"/>
-      <c r="C14" s="41"/>
+      <c r="C14" s="43"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -1808,80 +1808,80 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
+      <c r="B15" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="47"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="12" t="s">
+      <c r="B20" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="12" t="s">
-        <v>6</v>
+      <c r="F20" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1889,7 +1889,7 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B21" s="13"/>
-      <c r="C21" s="40"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
@@ -1900,7 +1900,7 @@
         <v>0.61458333333333304</v>
       </c>
       <c r="B22" s="13"/>
-      <c r="C22" s="40"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
@@ -1911,7 +1911,7 @@
         <v>0.625</v>
       </c>
       <c r="B23" s="14"/>
-      <c r="C23" s="41"/>
+      <c r="C23" s="43"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
@@ -1921,26 +1921,26 @@
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="4">
         <v>0.64583333333333304</v>
       </c>
       <c r="B25" s="13"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="33"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="28"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
@@ -1950,8 +1950,8 @@
         <v>0.65625</v>
       </c>
       <c r="B26" s="13"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="33"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="28"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
@@ -1961,8 +1961,8 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="B27" s="14"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="34"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="29"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -1971,26 +1971,26 @@
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
+      <c r="B28" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
       <c r="B29" s="13"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="33"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="28"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
@@ -2000,8 +2000,8 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="13"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="33"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="28"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
@@ -2011,8 +2011,8 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B31" s="14"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="34"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="29"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -2032,11 +2032,11 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="37" t="s">
-        <v>11</v>
+      <c r="B33" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -2048,7 +2048,7 @@
         <v>0.73958333333333104</v>
       </c>
       <c r="B34" s="13"/>
-      <c r="C34" s="40"/>
+      <c r="C34" s="42"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -2059,7 +2059,7 @@
         <v>0.749999999999997</v>
       </c>
       <c r="B35" s="13"/>
-      <c r="C35" s="40"/>
+      <c r="C35" s="42"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -2070,7 +2070,7 @@
         <v>0.76041666666666297</v>
       </c>
       <c r="B36" s="13"/>
-      <c r="C36" s="40"/>
+      <c r="C36" s="42"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2081,7 +2081,7 @@
         <v>0.77083333333332904</v>
       </c>
       <c r="B37" s="13"/>
-      <c r="C37" s="40"/>
+      <c r="C37" s="42"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -2092,7 +2092,7 @@
         <v>0.781249999999996</v>
       </c>
       <c r="B38" s="13"/>
-      <c r="C38" s="40"/>
+      <c r="C38" s="42"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -2103,7 +2103,7 @@
         <v>0.79166666666666197</v>
       </c>
       <c r="B39" s="14"/>
-      <c r="C39" s="41"/>
+      <c r="C39" s="43"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
@@ -2111,24 +2111,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
     <mergeCell ref="F28:F31"/>
     <mergeCell ref="G28:G31"/>
     <mergeCell ref="B33:B39"/>
@@ -2145,6 +2127,24 @@
     <mergeCell ref="G24:G27"/>
     <mergeCell ref="F7:F10"/>
     <mergeCell ref="G7:G10"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2154,8 +2154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4604F1AA-DEDD-4C2A-B2D1-8301823F4329}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2169,13 +2169,13 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2187,62 +2187,62 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
+      <c r="B3" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="12" t="s">
+      <c r="B7" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="26" t="s">
         <v>5</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2279,20 +2279,20 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>27</v>
+      <c r="B11" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2329,72 +2329,72 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
+      <c r="B15" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="47"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="12" t="s">
+      <c r="B20" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="C20" s="31" t="s">
         <v>4</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2431,16 +2431,16 @@
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="12"/>
+      <c r="E24" s="26"/>
       <c r="F24" s="10"/>
     </row>
     <row r="25" spans="1:6">
@@ -2477,16 +2477,16 @@
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="12"/>
+      <c r="E28" s="26"/>
       <c r="F28" s="10"/>
     </row>
     <row r="29" spans="1:6">
@@ -2494,7 +2494,7 @@
         <v>0.6875</v>
       </c>
       <c r="B29" s="13"/>
-      <c r="C29" s="33"/>
+      <c r="C29" s="28"/>
       <c r="D29" s="51"/>
       <c r="E29" s="13"/>
       <c r="F29" s="8"/>
@@ -2504,7 +2504,7 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="13"/>
-      <c r="C30" s="33"/>
+      <c r="C30" s="28"/>
       <c r="D30" s="51"/>
       <c r="E30" s="13"/>
       <c r="F30" s="8"/>
@@ -2514,7 +2514,7 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B31" s="14"/>
-      <c r="C31" s="34"/>
+      <c r="C31" s="29"/>
       <c r="D31" s="52"/>
       <c r="E31" s="14"/>
       <c r="F31" s="8"/>
@@ -2533,11 +2533,11 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="37" t="s">
-        <v>11</v>
+      <c r="B33" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -2605,17 +2605,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="B33:B39"/>
-    <mergeCell ref="C33:C39"/>
     <mergeCell ref="B3:F6"/>
     <mergeCell ref="B15:F19"/>
     <mergeCell ref="F20:F23"/>
@@ -2632,6 +2621,17 @@
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="C20:C23"/>
     <mergeCell ref="D20:D23"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="C33:C39"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2642,7 +2642,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:G10"/>
+      <selection activeCell="C20" sqref="C20:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2658,13 +2658,13 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2678,69 +2678,69 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
+      <c r="B3" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="12" t="s">
+      <c r="B7" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="G7" s="26" t="s">
         <v>6</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2748,7 +2748,7 @@
         <v>0.46875</v>
       </c>
       <c r="B8" s="13"/>
-      <c r="C8" s="33"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
@@ -2759,7 +2759,7 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B9" s="13"/>
-      <c r="C9" s="33"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -2770,7 +2770,7 @@
         <v>0.48958333333333298</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="34"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -2780,23 +2780,23 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>8</v>
+      <c r="B11" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2804,7 +2804,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="B12" s="13"/>
-      <c r="C12" s="33"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
@@ -2815,7 +2815,7 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B13" s="13"/>
-      <c r="C13" s="33"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
@@ -2826,7 +2826,7 @@
         <v>0.53125</v>
       </c>
       <c r="B14" s="14"/>
-      <c r="C14" s="34"/>
+      <c r="C14" s="29"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -2836,80 +2836,80 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
+      <c r="B15" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="47"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="19" t="s">
+      <c r="B20" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="33" t="s">
         <v>5</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="19" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2917,7 +2917,7 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B21" s="13"/>
-      <c r="C21" s="33"/>
+      <c r="C21" s="28"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
@@ -2928,7 +2928,7 @@
         <v>0.61458333333333304</v>
       </c>
       <c r="B22" s="13"/>
-      <c r="C22" s="33"/>
+      <c r="C22" s="28"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
@@ -2939,7 +2939,7 @@
         <v>0.625</v>
       </c>
       <c r="B23" s="14"/>
-      <c r="C23" s="34"/>
+      <c r="C23" s="29"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
@@ -2949,18 +2949,18 @@
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="4">
@@ -2968,7 +2968,7 @@
       </c>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="33"/>
+      <c r="D25" s="28"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
@@ -2979,7 +2979,7 @@
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="33"/>
+      <c r="D26" s="28"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
@@ -2990,7 +2990,7 @@
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
-      <c r="D27" s="34"/>
+      <c r="D27" s="29"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -2999,26 +2999,26 @@
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
       <c r="B29" s="13"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
@@ -3028,8 +3028,8 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="13"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
@@ -3039,8 +3039,8 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B31" s="14"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -3060,11 +3060,11 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="37" t="s">
-        <v>11</v>
+      <c r="B33" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -3139,27 +3139,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B33:B39"/>
-    <mergeCell ref="C33:C39"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="G28:G31"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="B15:G19"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="G20:G23"/>
     <mergeCell ref="G11:G14"/>
     <mergeCell ref="B3:G6"/>
     <mergeCell ref="B7:B10"/>
@@ -3173,6 +3152,27 @@
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="F11:F14"/>
+    <mergeCell ref="B15:G19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="C33:C39"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3182,8 +3182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82DEF69-E5FD-41F0-9622-94C4199D6A7C}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3196,13 +3196,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1">
@@ -3216,8 +3216,8 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="42" t="s">
-        <v>13</v>
+      <c r="B3" s="44" t="s">
+        <v>11</v>
       </c>
       <c r="C3" s="53"/>
       <c r="D3" s="53"/>
@@ -3228,34 +3228,34 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="B4" s="54"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
       <c r="B5" s="54"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
       <c r="B6" s="54"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C7" s="56"/>
       <c r="D7" s="56"/>
@@ -3328,55 +3328,55 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
+      <c r="B15" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
       <c r="B20" s="55" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C20" s="56"/>
       <c r="D20" s="56"/>
@@ -3413,16 +3413,16 @@
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="12"/>
+      <c r="E24" s="26"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="4">
@@ -3430,7 +3430,7 @@
       </c>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="33"/>
+      <c r="D25" s="28"/>
       <c r="E25" s="13"/>
     </row>
     <row r="26" spans="1:5">
@@ -3439,7 +3439,7 @@
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="33"/>
+      <c r="D26" s="28"/>
       <c r="E26" s="13"/>
     </row>
     <row r="27" spans="1:5">
@@ -3448,31 +3448,31 @@
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
-      <c r="D27" s="34"/>
+      <c r="D27" s="29"/>
       <c r="E27" s="14"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="12"/>
+      <c r="E28" s="26"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
       <c r="B29" s="13"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
       <c r="E29" s="13"/>
     </row>
     <row r="30" spans="1:5">
@@ -3480,8 +3480,8 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="13"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
       <c r="E30" s="13"/>
     </row>
     <row r="31" spans="1:5">
@@ -3489,8 +3489,8 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B31" s="14"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
       <c r="E31" s="14"/>
     </row>
     <row r="32" spans="1:5">
@@ -3506,11 +3506,11 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="37" t="s">
-        <v>11</v>
+      <c r="B33" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -3571,12 +3571,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="B33:B39"/>
-    <mergeCell ref="C33:C39"/>
     <mergeCell ref="B3:E6"/>
     <mergeCell ref="B7:E14"/>
     <mergeCell ref="B15:E19"/>
@@ -3585,6 +3579,12 @@
     <mergeCell ref="C24:C27"/>
     <mergeCell ref="D24:D27"/>
     <mergeCell ref="E24:E27"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="C33:C39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3595,7 +3595,7 @@
   <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3610,18 +3610,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1">
       <c r="A2" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B2" s="42" t="s">
-        <v>48</v>
+      <c r="B2" s="44" t="s">
+        <v>46</v>
       </c>
       <c r="C2" s="53"/>
     </row>
@@ -3630,354 +3630,354 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="B3" s="54"/>
-      <c r="C3" s="28"/>
+      <c r="C3" s="23"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4">
         <v>0.4375</v>
       </c>
       <c r="B4" s="54"/>
-      <c r="C4" s="28"/>
+      <c r="C4" s="23"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4">
         <v>0.44791666666666702</v>
       </c>
       <c r="B5" s="54"/>
-      <c r="C5" s="28"/>
+      <c r="C5" s="23"/>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1">
       <c r="A6" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B6" s="64" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="65"/>
+      <c r="B6" s="80" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="81"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="67"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="83"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="67"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="83"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="67"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="83"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4">
         <v>0.5</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="67"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="83"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="67"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="83"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B12" s="66"/>
-      <c r="C12" s="67"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="83"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B13" s="68"/>
-      <c r="C13" s="69"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="85"/>
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1">
       <c r="A14" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B14" s="70" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="71"/>
+      <c r="B14" s="86" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="87"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B15" s="72"/>
-      <c r="C15" s="16"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="37"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B16" s="72"/>
-      <c r="C16" s="16"/>
+      <c r="B16" s="88"/>
+      <c r="C16" s="37"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B17" s="72"/>
-      <c r="C17" s="16"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="37"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B18" s="72"/>
-      <c r="C18" s="16"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="37"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B19" s="72"/>
-      <c r="C19" s="16"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="37"/>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1">
       <c r="A20" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B20" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="65"/>
+      <c r="B20" s="80" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="81"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B21" s="66"/>
-      <c r="C21" s="67"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="83"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="4">
         <v>0.625</v>
       </c>
-      <c r="B22" s="66"/>
-      <c r="C22" s="67"/>
+      <c r="B22" s="82"/>
+      <c r="C22" s="83"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B23" s="66"/>
-      <c r="C23" s="67"/>
+      <c r="B23" s="82"/>
+      <c r="C23" s="83"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B24" s="66"/>
-      <c r="C24" s="67"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="83"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B25" s="66"/>
-      <c r="C25" s="67"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="83"/>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1">
       <c r="A26" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B26" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="74"/>
+      <c r="B26" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="65"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B27" s="75"/>
-      <c r="C27" s="76"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="67"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="4">
         <v>0.6875</v>
       </c>
-      <c r="B28" s="77"/>
-      <c r="C28" s="78"/>
+      <c r="B28" s="68"/>
+      <c r="C28" s="69"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="4">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B29" s="73" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="74"/>
+      <c r="B29" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="65"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="4">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B30" s="75"/>
-      <c r="C30" s="76"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="67"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B31" s="77"/>
-      <c r="C31" s="78"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="69"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B32" s="79" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="80"/>
+      <c r="B32" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="71"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B33" s="81"/>
-      <c r="C33" s="82"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="73"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B34" s="81"/>
-      <c r="C34" s="82"/>
+      <c r="B34" s="72"/>
+      <c r="C34" s="73"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B35" s="83"/>
-      <c r="C35" s="84"/>
+      <c r="B35" s="74"/>
+      <c r="C35" s="75"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B36" s="85" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="85"/>
+      <c r="B36" s="76" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="76"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B37" s="86"/>
-      <c r="C37" s="86"/>
+      <c r="B37" s="77"/>
+      <c r="C37" s="77"/>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="4">
         <v>0.79166666666666197</v>
       </c>
-      <c r="B38" s="86"/>
-      <c r="C38" s="86"/>
+      <c r="B38" s="77"/>
+      <c r="C38" s="77"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="4">
         <v>0.80208333333332804</v>
       </c>
-      <c r="B39" s="86"/>
-      <c r="C39" s="86"/>
+      <c r="B39" s="77"/>
+      <c r="C39" s="77"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="4">
         <v>0.812499999999994</v>
       </c>
-      <c r="B40" s="86"/>
-      <c r="C40" s="86"/>
+      <c r="B40" s="77"/>
+      <c r="C40" s="77"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="4">
         <v>0.82291666666665997</v>
       </c>
-      <c r="B41" s="79" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="80"/>
+      <c r="B41" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="71"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="4">
         <v>0.83333333333332604</v>
       </c>
-      <c r="B42" s="81"/>
-      <c r="C42" s="82"/>
+      <c r="B42" s="72"/>
+      <c r="C42" s="73"/>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="4">
         <v>0.84374999999999201</v>
       </c>
-      <c r="B43" s="81"/>
-      <c r="C43" s="82"/>
+      <c r="B43" s="72"/>
+      <c r="C43" s="73"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="4">
         <v>0.85416666666665797</v>
       </c>
-      <c r="B44" s="87" t="s">
-        <v>47</v>
-      </c>
-      <c r="C44" s="88"/>
+      <c r="B44" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="79"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="4">
         <v>0.86458333333332404</v>
       </c>
-      <c r="B45" s="77"/>
-      <c r="C45" s="78"/>
+      <c r="B45" s="68"/>
+      <c r="C45" s="69"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="4">
         <v>0.87499999999999001</v>
       </c>
-      <c r="B46" s="77"/>
-      <c r="C46" s="78"/>
+      <c r="B46" s="68"/>
+      <c r="C46" s="69"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="4">
         <v>0.88541666666665597</v>
       </c>
-      <c r="B47" s="77"/>
-      <c r="C47" s="78"/>
+      <c r="B47" s="68"/>
+      <c r="C47" s="69"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="4">
         <v>0.89583333333332205</v>
       </c>
-      <c r="B48" s="77"/>
-      <c r="C48" s="78"/>
+      <c r="B48" s="68"/>
+      <c r="C48" s="69"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="4">
         <v>0.90624999999998801</v>
       </c>
-      <c r="B49" s="77"/>
-      <c r="C49" s="78"/>
+      <c r="B49" s="68"/>
+      <c r="C49" s="69"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="4">
         <v>0.91666666666665497</v>
       </c>
-      <c r="B50" s="77"/>
-      <c r="C50" s="78"/>
+      <c r="B50" s="68"/>
+      <c r="C50" s="69"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="4">
@@ -4016,16 +4016,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:C5"/>
+    <mergeCell ref="B6:C13"/>
+    <mergeCell ref="B14:C19"/>
+    <mergeCell ref="B20:C25"/>
+    <mergeCell ref="B26:C28"/>
     <mergeCell ref="B29:C31"/>
     <mergeCell ref="B32:C35"/>
     <mergeCell ref="B36:C40"/>
     <mergeCell ref="B41:C43"/>
     <mergeCell ref="B44:C50"/>
-    <mergeCell ref="B2:C5"/>
-    <mergeCell ref="B6:C13"/>
-    <mergeCell ref="B14:C19"/>
-    <mergeCell ref="B20:C25"/>
-    <mergeCell ref="B26:C28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove outdated student timetable files and enhance timetable generation logic to ensure room information is displayed correctly in activity descriptions.
</commit_message>
<xml_diff>
--- a/flute-time-table.xlsx
+++ b/flute-time-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmski\Desktop\Timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACE39A4-69D2-46EB-B6CD-9363A4AAD6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1145763-AC6B-4ED0-A5CD-341F766A067C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="2" xr2:uid="{4F305ACA-9255-4D6C-9A65-1407DE2CF383}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="4" xr2:uid="{4F305ACA-9255-4D6C-9A65-1407DE2CF383}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="51">
   <si>
     <t xml:space="preserve">Time </t>
   </si>
@@ -149,9 +149,6 @@
   <si>
     <t>Briefing for Saturday
 (Room zzz)</t>
-  </si>
-  <si>
-    <t>Flute MasterClass</t>
   </si>
   <si>
     <t>Check in Maritime Museum
@@ -191,10 +188,6 @@
 (Room Acting Class)</t>
   </si>
   <si>
-    <t>Group Activity
-(Room Group Activity)</t>
-  </si>
-  <si>
     <t>F4 Rehearsal with pianist
 (Room Shelley)</t>
   </si>
@@ -209,6 +202,18 @@
   <si>
     <t>Group 7
 (Room Liya)</t>
+  </si>
+  <si>
+    <t>Flute MasterClass
+(Room Stephane)</t>
+  </si>
+  <si>
+    <t>Group 2, 5, 8, 9 Group Activity
+(Room Group Activity)</t>
+  </si>
+  <si>
+    <t>Group 1, 3, 4, 6, 7 Group Activity
+(Room Group Activity)</t>
   </si>
 </sst>
 </file>
@@ -581,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -601,12 +606,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -800,6 +799,24 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -817,9 +834,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -827,10 +841,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1210,68 +1221,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1279,55 +1290,55 @@
       <c r="A8" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="14" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1335,101 +1346,101 @@
       <c r="A12" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="14" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1437,140 +1448,140 @@
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="29" t="s">
+      <c r="D23" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F23" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="16"/>
+      <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="13"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="13"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="14"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="29" t="s">
+      <c r="D27" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
@@ -1583,10 +1594,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="38" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1594,43 +1605,43 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="4">
@@ -1712,68 +1723,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="17" t="s">
+      <c r="C7" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="15" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1781,55 +1792,55 @@
       <c r="A8" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="16" t="s">
+      <c r="C11" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="14" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1837,101 +1848,101 @@
       <c r="A12" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="50"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="48"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="51"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="52"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="52"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="50"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="53"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="55"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="53"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="17" t="s">
+      <c r="C19" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="15" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1939,140 +1950,140 @@
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C23" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="29" t="s">
+      <c r="D23" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F23" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="16"/>
+      <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="13"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="13"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="14"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="29" t="s">
+      <c r="D27" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
@@ -2089,10 +2100,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="38" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="7"/>
@@ -2104,8 +2115,8 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="45"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="43"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -2115,8 +2126,8 @@
       <c r="A34" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="45"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="43"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -2126,8 +2137,8 @@
       <c r="A35" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="45"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="43"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -2137,8 +2148,8 @@
       <c r="A36" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="45"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="43"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2148,8 +2159,8 @@
       <c r="A37" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="45"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="43"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -2159,8 +2170,8 @@
       <c r="A38" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="46"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="44"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -2216,7 +2227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4604F1AA-DEDD-4C2A-B2D1-8301823F4329}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23:B26"/>
     </sheetView>
   </sheetViews>
@@ -2246,68 +2257,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="64"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="62"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="15" t="s">
+      <c r="D7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2315,55 +2326,55 @@
       <c r="A8" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="59"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="15" t="s">
+      <c r="D11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="13" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2371,101 +2382,101 @@
       <c r="A12" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B14" s="60"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="66"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="64"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="51"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="52"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="52"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="50"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="69"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="67"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="15" t="s">
+      <c r="D19" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="13" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2473,140 +2484,140 @@
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="59"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B22" s="60"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="70" t="s">
+      <c r="B23" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="29" t="s">
+      <c r="D23" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="G23" s="15"/>
+      <c r="F23" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="71"/>
-      <c r="C24" s="76"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="13"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="71"/>
-      <c r="C25" s="76"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="13"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="75"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="14"/>
+      <c r="B26" s="73"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="70" t="s">
+      <c r="B27" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="29" t="s">
+      <c r="D27" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="71"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="71"/>
-      <c r="C29" s="73"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="B29" s="69"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="72"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="72"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
@@ -2623,10 +2634,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="38" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="7"/>
@@ -2638,8 +2649,8 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="56"/>
-      <c r="C33" s="56"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -2649,8 +2660,8 @@
       <c r="A34" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="56"/>
-      <c r="C34" s="56"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="54"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -2660,8 +2671,8 @@
       <c r="A35" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="56"/>
-      <c r="C35" s="56"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="54"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -2671,8 +2682,8 @@
       <c r="A36" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="56"/>
-      <c r="C36" s="56"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="54"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2682,8 +2693,8 @@
       <c r="A37" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="56"/>
-      <c r="C37" s="56"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -2693,8 +2704,8 @@
       <c r="A38" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="57"/>
-      <c r="C38" s="57"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="55"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -2782,68 +2793,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="38" t="s">
+      <c r="C7" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="36" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2851,55 +2862,55 @@
       <c r="A8" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="15" t="s">
+      <c r="C11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2907,101 +2918,101 @@
       <c r="A12" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="50"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="48"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="51"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="52"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="52"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="50"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="53"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="55"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="53"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="15" t="s">
+      <c r="C19" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="13" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3009,140 +3020,140 @@
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="29" t="s">
+      <c r="D23" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F23" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="15"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="13"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="13"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="14"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="29" t="s">
+      <c r="D27" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
@@ -3159,10 +3170,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="38" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="5"/>
@@ -3174,8 +3185,8 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -3185,8 +3196,8 @@
       <c r="A34" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -3196,8 +3207,8 @@
       <c r="A35" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -3207,8 +3218,8 @@
       <c r="A36" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -3218,8 +3229,8 @@
       <c r="A37" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -3229,8 +3240,8 @@
       <c r="A38" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -3286,8 +3297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82DEF69-E5FD-41F0-9622-94C4199D6A7C}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:D30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3318,227 +3329,227 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="80"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="84"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="83"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="87"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="83"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="87"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="81"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="83"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="87"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="84" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="86"/>
+      <c r="B7" s="76" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="89"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B8" s="84"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="86"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="89"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="84"/>
-      <c r="C9" s="85"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="86"/>
+      <c r="B9" s="90"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="89"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="86"/>
+      <c r="B10" s="90"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="89"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="84"/>
-      <c r="C11" s="85"/>
-      <c r="D11" s="85"/>
-      <c r="E11" s="85"/>
-      <c r="F11" s="86"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="89"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B12" s="84"/>
-      <c r="C12" s="85"/>
-      <c r="D12" s="85"/>
-      <c r="E12" s="85"/>
-      <c r="F12" s="86"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="89"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B13" s="84"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="85"/>
-      <c r="F13" s="86"/>
+      <c r="B13" s="90"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="89"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B14" s="84"/>
-      <c r="C14" s="85"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="85"/>
-      <c r="F14" s="86"/>
+      <c r="B14" s="90"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="89"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="52"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="50"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="51"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="52"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="50"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="52"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="50"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="52"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B18" s="49"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="50"/>
+    </row>
+    <row r="19" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="84" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="85"/>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85"/>
-      <c r="F19" s="9"/>
+      <c r="B19" s="76" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="77"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="78"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="84"/>
-      <c r="C20" s="85"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="85"/>
-      <c r="F20" s="9"/>
+      <c r="B20" s="76"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="78"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B21" s="84"/>
-      <c r="C21" s="85"/>
-      <c r="D21" s="85"/>
-      <c r="E21" s="85"/>
-      <c r="F21" s="9"/>
+      <c r="B21" s="76"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="78"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B22" s="87"/>
-      <c r="C22" s="88"/>
-      <c r="D22" s="88"/>
-      <c r="E22" s="88"/>
-      <c r="F22" s="10"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B22" s="79"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="81"/>
+    </row>
+    <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="76" t="s">
+      <c r="B23" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="76" t="s">
+      <c r="C23" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="89" t="s">
+      <c r="D23" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="89" t="s">
+      <c r="F23" s="91" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3546,79 +3557,79 @@
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+    </row>
+    <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="29" t="s">
+      <c r="D27" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="15"/>
+      <c r="F27" s="13"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="13"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="13"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="14"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="12"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
@@ -3634,10 +3645,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="38" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="7"/>
@@ -3648,8 +3659,8 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="56"/>
-      <c r="C33" s="13"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="11"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -3658,8 +3669,8 @@
       <c r="A34" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="56"/>
-      <c r="C34" s="13"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="11"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -3668,8 +3679,8 @@
       <c r="A35" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="56"/>
-      <c r="C35" s="13"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="11"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -3678,8 +3689,8 @@
       <c r="A36" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="56"/>
-      <c r="C36" s="13"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="11"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -3688,8 +3699,8 @@
       <c r="A37" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="56"/>
-      <c r="C37" s="13"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="11"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -3698,8 +3709,8 @@
       <c r="A38" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="57"/>
-      <c r="C38" s="14"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="12"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -3711,12 +3722,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B19:F22"/>
     <mergeCell ref="B32:B38"/>
     <mergeCell ref="C32:C38"/>
     <mergeCell ref="B3:F6"/>
     <mergeCell ref="B7:F14"/>
     <mergeCell ref="B15:F18"/>
-    <mergeCell ref="B19:E22"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="C23:C26"/>
     <mergeCell ref="D23:D26"/>
@@ -3756,83 +3767,83 @@
       <c r="A2" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B2" s="90" t="s">
-        <v>34</v>
+      <c r="B2" s="92" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B3" s="90"/>
+      <c r="B3" s="92"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B4" s="90"/>
+      <c r="B4" s="92"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B5" s="90"/>
+      <c r="B5" s="92"/>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B6" s="91" t="s">
-        <v>35</v>
+      <c r="B6" s="93" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B7" s="91"/>
+      <c r="B7" s="93"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B8" s="91"/>
+      <c r="B8" s="93"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B9" s="91"/>
+      <c r="B9" s="93"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>0.5</v>
       </c>
-      <c r="B10" s="91"/>
+      <c r="B10" s="93"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B11" s="91"/>
+      <c r="B11" s="93"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B12" s="91"/>
+      <c r="B12" s="93"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B13" s="91"/>
+      <c r="B13" s="93"/>
     </row>
     <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B14" s="90" t="s">
+      <c r="B14" s="92" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3840,33 +3851,33 @@
       <c r="A15" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B15" s="90"/>
+      <c r="B15" s="92"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B16" s="90"/>
+      <c r="B16" s="92"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B17" s="90"/>
+      <c r="B17" s="92"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>36</v>
+      <c r="B18" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B19" s="91" t="s">
+      <c r="B19" s="93" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3874,37 +3885,37 @@
       <c r="A20" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B20" s="91"/>
+      <c r="B20" s="93"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B21" s="91"/>
+      <c r="B21" s="93"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>0.625</v>
       </c>
-      <c r="B22" s="91"/>
+      <c r="B22" s="93"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B23" s="91"/>
+      <c r="B23" s="93"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B24" s="91"/>
+      <c r="B24" s="93"/>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B25" s="91" t="s">
+      <c r="B25" s="93" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3912,13 +3923,13 @@
       <c r="A26" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B26" s="91"/>
+      <c r="B26" s="93"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B27" s="91"/>
+      <c r="B27" s="93"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" s="4">

</xml_diff>

<commit_message>
Refine timetable generation logic to improve activity descriptions for private lessons and group activities, ensuring accurate representation of room information and handling of cleaned activity text.
</commit_message>
<xml_diff>
--- a/flute-time-table.xlsx
+++ b/flute-time-table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmski\Desktop\Timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1145763-AC6B-4ED0-A5CD-341F766A067C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB416A28-8686-4525-8BCD-C3088381092E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="4" xr2:uid="{4F305ACA-9255-4D6C-9A65-1407DE2CF383}"/>
   </bookViews>
@@ -609,19 +609,63 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -653,60 +697,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -733,11 +727,59 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -751,53 +793,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1189,7 +1189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58029A68-0D30-435A-A4C3-6E59A3275874}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D27" sqref="D27:D30"/>
     </sheetView>
   </sheetViews>
@@ -1221,68 +1221,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="35"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="38"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="38"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="41"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="24" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1323,22 +1323,22 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1349,7 +1349,7 @@
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="15"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
     </row>
@@ -1360,7 +1360,7 @@
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
-      <c r="E13" s="15"/>
+      <c r="E13" s="24"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
     </row>
@@ -1371,7 +1371,7 @@
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
-      <c r="E14" s="16"/>
+      <c r="E14" s="32"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
@@ -1379,68 +1379,68 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1481,22 +1481,22 @@
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="14"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
@@ -1504,9 +1504,9 @@
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
@@ -1515,9 +1515,9 @@
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
@@ -1526,38 +1526,38 @@
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C27" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
       <c r="B28" s="11"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="28"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
     </row>
@@ -1566,9 +1566,9 @@
         <v>0.6875</v>
       </c>
       <c r="B29" s="11"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="28"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
     </row>
@@ -1577,9 +1577,9 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="12"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="29"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="21"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
     </row>
@@ -1594,10 +1594,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="13" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1650,14 +1650,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="B7:B10"/>
     <mergeCell ref="E23:E26"/>
     <mergeCell ref="F23:F26"/>
     <mergeCell ref="G23:G26"/>
@@ -1674,16 +1676,14 @@
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="C23:C26"/>
     <mergeCell ref="D23:D26"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1723,68 +1723,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="35"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="38"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="38"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="41"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="24" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1793,7 +1793,7 @@
         <v>0.46875</v>
       </c>
       <c r="B8" s="11"/>
-      <c r="C8" s="43"/>
+      <c r="C8" s="42"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -1804,7 +1804,7 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="43"/>
+      <c r="C9" s="42"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -1815,7 +1815,7 @@
         <v>0.48958333333333298</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="44"/>
+      <c r="C10" s="43"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -1825,22 +1825,22 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1849,7 +1849,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="C12" s="43"/>
+      <c r="C12" s="42"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -1860,7 +1860,7 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B13" s="11"/>
-      <c r="C13" s="43"/>
+      <c r="C13" s="42"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
@@ -1871,7 +1871,7 @@
         <v>0.53125</v>
       </c>
       <c r="B14" s="11"/>
-      <c r="C14" s="43"/>
+      <c r="C14" s="42"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -1881,68 +1881,68 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="48"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="46"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="50"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="50"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="48"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="53"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="51"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="24" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1951,7 +1951,7 @@
         <v>0.59375</v>
       </c>
       <c r="B20" s="11"/>
-      <c r="C20" s="43"/>
+      <c r="C20" s="42"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
@@ -1962,7 +1962,7 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="43"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
@@ -1973,7 +1973,7 @@
         <v>0.61458333333333304</v>
       </c>
       <c r="B22" s="12"/>
-      <c r="C22" s="44"/>
+      <c r="C22" s="43"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
@@ -1983,32 +1983,32 @@
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="14"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
       <c r="B24" s="11"/>
-      <c r="C24" s="43"/>
+      <c r="C24" s="42"/>
       <c r="D24" s="11"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
@@ -2016,10 +2016,10 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B25" s="11"/>
-      <c r="C25" s="43"/>
+      <c r="C25" s="42"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
@@ -2027,39 +2027,39 @@
         <v>0.65625</v>
       </c>
       <c r="B26" s="12"/>
-      <c r="C26" s="44"/>
+      <c r="C26" s="43"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C27" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
       <c r="B28" s="11"/>
-      <c r="C28" s="40"/>
+      <c r="C28" s="16"/>
       <c r="D28" s="11"/>
-      <c r="E28" s="28"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
     </row>
@@ -2068,9 +2068,9 @@
         <v>0.6875</v>
       </c>
       <c r="B29" s="11"/>
-      <c r="C29" s="40"/>
+      <c r="C29" s="16"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="28"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
     </row>
@@ -2079,9 +2079,9 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="12"/>
-      <c r="C30" s="41"/>
+      <c r="C30" s="17"/>
       <c r="D30" s="12"/>
-      <c r="E30" s="29"/>
+      <c r="E30" s="21"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
     </row>
@@ -2100,10 +2100,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="7"/>
@@ -2116,7 +2116,7 @@
         <v>0.72916666666666496</v>
       </c>
       <c r="B33" s="11"/>
-      <c r="C33" s="43"/>
+      <c r="C33" s="42"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -2127,7 +2127,7 @@
         <v>0.73958333333333104</v>
       </c>
       <c r="B34" s="11"/>
-      <c r="C34" s="43"/>
+      <c r="C34" s="42"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -2138,7 +2138,7 @@
         <v>0.749999999999997</v>
       </c>
       <c r="B35" s="11"/>
-      <c r="C35" s="43"/>
+      <c r="C35" s="42"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -2149,7 +2149,7 @@
         <v>0.76041666666666297</v>
       </c>
       <c r="B36" s="11"/>
-      <c r="C36" s="43"/>
+      <c r="C36" s="42"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2160,7 +2160,7 @@
         <v>0.77083333333332904</v>
       </c>
       <c r="B37" s="11"/>
-      <c r="C37" s="43"/>
+      <c r="C37" s="42"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -2171,7 +2171,7 @@
         <v>0.781249999999996</v>
       </c>
       <c r="B38" s="12"/>
-      <c r="C38" s="44"/>
+      <c r="C38" s="43"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -2184,6 +2184,26 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="B15:G18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="G19:G22"/>
     <mergeCell ref="B32:B38"/>
     <mergeCell ref="C32:C38"/>
     <mergeCell ref="F23:F26"/>
@@ -2198,26 +2218,6 @@
     <mergeCell ref="C23:C26"/>
     <mergeCell ref="D23:D26"/>
     <mergeCell ref="E23:E26"/>
-    <mergeCell ref="B15:G18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2228,7 +2228,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:B26"/>
+      <selection activeCell="B3" sqref="B3:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2257,68 +2257,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="35"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="38"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="38"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="62"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="64"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="18" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2326,8 +2326,8 @@
       <c r="A8" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -2337,8 +2337,8 @@
       <c r="A9" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="26"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="22"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -2348,8 +2348,8 @@
       <c r="A10" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="59"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="73"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -2359,22 +2359,22 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="18" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2382,8 +2382,8 @@
       <c r="A12" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B12" s="57"/>
-      <c r="C12" s="26"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -2393,8 +2393,8 @@
       <c r="A13" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="26"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
@@ -2404,8 +2404,8 @@
       <c r="A14" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B14" s="58"/>
-      <c r="C14" s="59"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="73"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -2415,68 +2415,68 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="64"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="66"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="50"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="50"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="48"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="65"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="67"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="69"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="18" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2484,8 +2484,8 @@
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="26"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
@@ -2495,8 +2495,8 @@
       <c r="A21" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B21" s="57"/>
-      <c r="C21" s="26"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="22"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
@@ -2506,8 +2506,8 @@
       <c r="A22" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B22" s="58"/>
-      <c r="C22" s="59"/>
+      <c r="B22" s="72"/>
+      <c r="C22" s="73"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
@@ -2517,83 +2517,83 @@
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="68" t="s">
+      <c r="B23" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G23" s="13"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="69"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="69"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="73"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="68" t="s">
+      <c r="B27" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C27" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="69"/>
-      <c r="C28" s="71"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="28"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
     </row>
@@ -2601,10 +2601,10 @@
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="69"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="28"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
     </row>
@@ -2612,10 +2612,10 @@
       <c r="A30" s="4">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="70"/>
-      <c r="C30" s="72"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="29"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="21"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
     </row>
@@ -2634,10 +2634,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="7"/>
@@ -2649,8 +2649,8 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="54"/>
-      <c r="C33" s="54"/>
+      <c r="B33" s="74"/>
+      <c r="C33" s="74"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -2660,8 +2660,8 @@
       <c r="A34" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="54"/>
-      <c r="C34" s="54"/>
+      <c r="B34" s="74"/>
+      <c r="C34" s="74"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -2671,8 +2671,8 @@
       <c r="A35" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="54"/>
-      <c r="C35" s="54"/>
+      <c r="B35" s="74"/>
+      <c r="C35" s="74"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -2682,8 +2682,8 @@
       <c r="A36" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="54"/>
-      <c r="C36" s="54"/>
+      <c r="B36" s="74"/>
+      <c r="C36" s="74"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2693,8 +2693,8 @@
       <c r="A37" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="54"/>
-      <c r="C37" s="54"/>
+      <c r="B37" s="74"/>
+      <c r="C37" s="74"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -2704,8 +2704,8 @@
       <c r="A38" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="55"/>
-      <c r="C38" s="55"/>
+      <c r="B38" s="75"/>
+      <c r="C38" s="75"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -2718,17 +2718,15 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="F23:F26"/>
     <mergeCell ref="B3:G6"/>
     <mergeCell ref="G7:G10"/>
     <mergeCell ref="G11:G14"/>
@@ -2743,15 +2741,17 @@
     <mergeCell ref="C7:C10"/>
     <mergeCell ref="D7:D10"/>
     <mergeCell ref="E7:E10"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2761,7 +2761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D66C3A2-B766-4AEA-9D50-70BB9454FECE}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D27" sqref="D27:D30"/>
     </sheetView>
   </sheetViews>
@@ -2793,68 +2793,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="35"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="38"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="38"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="41"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G7" s="30" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2863,7 +2863,7 @@
         <v>0.46875</v>
       </c>
       <c r="B8" s="11"/>
-      <c r="C8" s="40"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -2874,7 +2874,7 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="40"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -2885,7 +2885,7 @@
         <v>0.48958333333333298</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="41"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -2895,22 +2895,22 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2919,7 +2919,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="C12" s="40"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -2930,7 +2930,7 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B13" s="11"/>
-      <c r="C13" s="40"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
@@ -2941,7 +2941,7 @@
         <v>0.53125</v>
       </c>
       <c r="B14" s="11"/>
-      <c r="C14" s="40"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -2951,68 +2951,68 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="48"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="46"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="50"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="50"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="48"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="53"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="51"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="18" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3021,7 +3021,7 @@
         <v>0.59375</v>
       </c>
       <c r="B20" s="11"/>
-      <c r="C20" s="40"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
@@ -3032,7 +3032,7 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="40"/>
+      <c r="C21" s="16"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
@@ -3043,7 +3043,7 @@
         <v>0.61458333333333304</v>
       </c>
       <c r="B22" s="12"/>
-      <c r="C22" s="41"/>
+      <c r="C22" s="17"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
@@ -3053,22 +3053,22 @@
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="13"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
@@ -3077,8 +3077,8 @@
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
@@ -3088,8 +3088,8 @@
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
@@ -3099,37 +3099,37 @@
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C27" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
       <c r="B28" s="11"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="28"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
     </row>
@@ -3138,9 +3138,9 @@
         <v>0.6875</v>
       </c>
       <c r="B29" s="11"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="28"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
     </row>
@@ -3149,9 +3149,9 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="12"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="29"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="21"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
     </row>
@@ -3170,10 +3170,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="5"/>
@@ -3254,11 +3254,19 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
     <mergeCell ref="G23:G26"/>
     <mergeCell ref="E27:E30"/>
     <mergeCell ref="B15:G18"/>
@@ -3275,19 +3283,11 @@
     <mergeCell ref="F23:F26"/>
     <mergeCell ref="F27:F30"/>
     <mergeCell ref="G27:G30"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3453,43 +3453,43 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="50"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="48"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="50"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="48"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="50"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="48"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="49"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="50"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="48"/>
     </row>
     <row r="19" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
@@ -3537,13 +3537,13 @@
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="74" t="s">
+      <c r="B23" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="74" t="s">
+      <c r="C23" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="36" t="s">
+      <c r="D23" s="30" t="s">
         <v>49</v>
       </c>
       <c r="E23" s="91" t="s">
@@ -3559,9 +3559,9 @@
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
@@ -3569,9 +3569,9 @@
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
@@ -3579,36 +3579,36 @@
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
     </row>
     <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C27" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="13"/>
+      <c r="F27" s="18"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
       <c r="B28" s="11"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="28"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
@@ -3616,9 +3616,9 @@
         <v>0.6875</v>
       </c>
       <c r="B29" s="11"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="28"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -3626,9 +3626,9 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="12"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="29"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="21"/>
       <c r="F30" s="12"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
@@ -3645,10 +3645,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="7"/>
@@ -3659,7 +3659,7 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="54"/>
+      <c r="B33" s="74"/>
       <c r="C33" s="11"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -3669,7 +3669,7 @@
       <c r="A34" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="54"/>
+      <c r="B34" s="74"/>
       <c r="C34" s="11"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -3679,7 +3679,7 @@
       <c r="A35" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="54"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="11"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -3689,7 +3689,7 @@
       <c r="A36" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="54"/>
+      <c r="B36" s="74"/>
       <c r="C36" s="11"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -3699,7 +3699,7 @@
       <c r="A37" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="54"/>
+      <c r="B37" s="74"/>
       <c r="C37" s="11"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -3709,7 +3709,7 @@
       <c r="A38" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="55"/>
+      <c r="B38" s="75"/>
       <c r="C38" s="12"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>

</xml_diff>